<commit_message>
add self assessment manikins more consistent cue prompt separate C and NC conditions use IAPS pictures, make them big, and with constant size
</commit_message>
<xml_diff>
--- a/input_data/diamond_task/trial_list_S1_C_with_images.xlsx
+++ b/input_data/diamond_task/trial_list_S1_C_with_images.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="37">
   <si>
     <t>trial no.</t>
   </si>
@@ -117,115 +117,16 @@
     <t>Correct</t>
   </si>
   <si>
-    <t>amusement_0500.jpg</t>
+    <t>1710.JPG</t>
   </si>
   <si>
-    <t>amusement_0501.jpg</t>
+    <t>1022.JPG</t>
   </si>
   <si>
-    <t>amusement_0502.jpg</t>
-  </si>
-  <si>
-    <t>amusement_0503.jpg</t>
-  </si>
-  <si>
-    <t>amusement_0504.jpg</t>
-  </si>
-  <si>
-    <t>amusement_0505.jpg</t>
-  </si>
-  <si>
-    <t>amusement_0506.jpg</t>
-  </si>
-  <si>
-    <t>amusement_0507.jpg</t>
+    <t>1030.JPG</t>
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>anger_0800.jpg</t>
-  </si>
-  <si>
-    <t>anger_0801.jpg</t>
-  </si>
-  <si>
-    <t>anger_0802.jpg</t>
-  </si>
-  <si>
-    <t>anger_0803.jpg</t>
-  </si>
-  <si>
-    <t>anger_0804.jpg</t>
-  </si>
-  <si>
-    <t>anger_0806.jpg</t>
-  </si>
-  <si>
-    <t>anger_0807.jpg</t>
-  </si>
-  <si>
-    <t>anger_0808.jpg</t>
-  </si>
-  <si>
-    <t>anger_0809.jpg</t>
-  </si>
-  <si>
-    <t>awe_0590.jpg</t>
-  </si>
-  <si>
-    <t>awe_0591.jpg</t>
-  </si>
-  <si>
-    <t>awe_0592.jpg</t>
-  </si>
-  <si>
-    <t>awe_0593.jpg</t>
-  </si>
-  <si>
-    <t>awe_0594.jpg</t>
-  </si>
-  <si>
-    <t>awe_0595.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0090.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0091.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0092.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0093.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0094.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0095.jpg</t>
-  </si>
-  <si>
-    <t>contentment_0096.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0760.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0761.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0763.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0764.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0765.jpg</t>
-  </si>
-  <si>
-    <t>disgust_0766.jpg</t>
   </si>
 </sst>
 </file>
@@ -243,7 +144,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -312,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -334,6 +235,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -650,7 +554,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="41.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
@@ -663,13 +567,13 @@
     <col min="12" max="12" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="7" width="25.862142857142857" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="7" width="26.433571428571426" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="7" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="7" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="8" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -905,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -962,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1019,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1076,7 +980,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -1133,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -1154,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -1190,7 +1094,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -1247,7 +1151,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1304,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -1361,7 +1265,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1418,7 +1322,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1475,7 +1379,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1532,7 +1436,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1589,7 +1493,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1646,7 +1550,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1703,7 +1607,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1760,7 +1664,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1817,7 +1721,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1874,7 +1778,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -1931,7 +1835,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1988,7 +1892,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -2045,7 +1949,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -2102,7 +2006,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -2159,7 +2063,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -2216,7 +2120,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -2273,7 +2177,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -2330,7 +2234,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -2387,7 +2291,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -2444,7 +2348,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -2501,7 +2405,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -2558,7 +2462,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -2615,7 +2519,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -2672,7 +2576,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
@@ -2729,7 +2633,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -2797,55 +2701,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8">
+      <c r="B1" s="9">
         <v>0.71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>0.69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="9">
         <v>0.67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>0.65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="9">
         <v>0.62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="9">
         <v>0.6</v>
       </c>
     </row>
@@ -2867,11 +2771,11 @@
   <cols>
     <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="26.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="26.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
@@ -2883,7 +2787,7 @@
     <col min="16" max="16" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2923,7 +2827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2961,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2999,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3037,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3075,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3113,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3151,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3189,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3227,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3265,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3303,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3341,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3379,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3417,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3455,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3493,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3531,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3569,7 +3473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3607,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3645,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3683,7 +3587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3721,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3759,7 +3663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3797,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3835,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3873,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3911,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3949,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3987,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4025,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4063,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4101,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4139,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4177,7 +4081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4215,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4253,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1">
         <v>36</v>
       </c>

</xml_diff>